<commit_message>
Creacion BOM Conectores y EDCPSU MK2
</commit_message>
<xml_diff>
--- a/02.Hardware/MK2 PCBs/01.EDCPSU/BOM/EDCPSU_MK2_BOM.xlsx
+++ b/02.Hardware/MK2 PCBs/01.EDCPSU/BOM/EDCPSU_MK2_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reozen/Team Dropbox/David Garrido/MUSOTOKU/PROJECTS/MK2/01.Documentation/02.Fabricacion/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Javi\Team Dropbox\JRODRIGUEZ\Repositorios\07.MK2\02.Hardware\MK2 PCBs\01.EDCPSU\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{915C07E6-9F48-5F4F-8092-5FF6A7C6DAA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{607435AA-BB52-4939-9998-F438B356BC90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EDCPSUMK2" sheetId="1" r:id="rId1"/>
@@ -1850,7 +1850,7 @@
     <xf numFmtId="9" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2089,6 +2089,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="84" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="46" fillId="38" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -2098,96 +2101,96 @@
     <xf numFmtId="0" fontId="46" fillId="38" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="84" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="85">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Énfasis1 2" xfId="60" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Énfasis2 2" xfId="64" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
     <cellStyle name="20% - Énfasis3 2" xfId="68" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="20% - Énfasis4" xfId="31" builtinId="42" customBuiltin="1"/>
     <cellStyle name="20% - Énfasis4 2" xfId="72" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="20% - Énfasis5" xfId="35" builtinId="46" customBuiltin="1"/>
     <cellStyle name="20% - Énfasis5 2" xfId="76" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="20% - Énfasis6" xfId="39" builtinId="50" customBuiltin="1"/>
     <cellStyle name="20% - Énfasis6 2" xfId="80" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis1" xfId="20" builtinId="31" customBuiltin="1"/>
     <cellStyle name="40% - Énfasis1 2" xfId="61" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="40% - Énfasis2" xfId="24" builtinId="35" customBuiltin="1"/>
     <cellStyle name="40% - Énfasis2 2" xfId="65" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="40% - Énfasis3" xfId="28" builtinId="39" customBuiltin="1"/>
     <cellStyle name="40% - Énfasis3 2" xfId="69" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="40% - Énfasis4" xfId="32" builtinId="43" customBuiltin="1"/>
     <cellStyle name="40% - Énfasis4 2" xfId="73" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
     <cellStyle name="40% - Énfasis5 2" xfId="77" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
     <cellStyle name="40% - Énfasis6 2" xfId="81" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
     <cellStyle name="60% - Énfasis1 2" xfId="62" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
     <cellStyle name="60% - Énfasis2 2" xfId="66" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
+    <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
     <cellStyle name="60% - Énfasis3 2" xfId="70" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
     <cellStyle name="60% - Énfasis4 2" xfId="74" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
+    <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
     <cellStyle name="60% - Énfasis5 2" xfId="78" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
+    <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
     <cellStyle name="60% - Énfasis6 2" xfId="82" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Buena 2" xfId="47" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Bueno" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Cálculo 2" xfId="52" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
+    <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Celda de comprobación 2" xfId="54" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+    <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Celda vinculada 2" xfId="53" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Encabezado 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Encabezado 4" xfId="5" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Encabezado 4 2" xfId="46" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
+    <cellStyle name="Énfasis1" xfId="18" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Énfasis1 2" xfId="59" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
+    <cellStyle name="Énfasis2" xfId="22" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Énfasis2 2" xfId="63" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
+    <cellStyle name="Énfasis3" xfId="26" builtinId="37" customBuiltin="1"/>
     <cellStyle name="Énfasis3 2" xfId="67" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
+    <cellStyle name="Énfasis4" xfId="30" builtinId="41" customBuiltin="1"/>
     <cellStyle name="Énfasis4 2" xfId="71" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
+    <cellStyle name="Énfasis5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Énfasis5 2" xfId="75" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
+    <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Énfasis6 2" xfId="79" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
+    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Entrada 2" xfId="50" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="84" builtinId="8"/>
+    <cellStyle name="Hipervínculo" xfId="84" builtinId="8"/>
+    <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Incorrecto 2" xfId="48" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Neutral 2" xfId="49" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="42" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
+    <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Notas 2" xfId="56" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Porcentaje 2" xfId="83" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
+    <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Salida 2" xfId="51" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
+    <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Texto de advertencia 2" xfId="55" xr:uid="{00000000-0005-0000-0000-000049000000}"/>
+    <cellStyle name="Texto explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Texto explicativo 2" xfId="57" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Título 1 2" xfId="43" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
+    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Título 2 2" xfId="44" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
+    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Título 3 2" xfId="45" xr:uid="{00000000-0005-0000-0000-000052000000}"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Total 2" xfId="58" xr:uid="{00000000-0005-0000-0000-000054000000}"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -2226,7 +2229,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2548,40 +2551,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
-      <selection activeCell="E86" sqref="E86"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" style="18" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" style="30" customWidth="1"/>
-    <col min="4" max="4" width="5.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="36.5" style="10" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="18" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="30" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="38.7109375" style="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="39" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="49.5" customWidth="1"/>
-    <col min="10" max="10" width="27.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="11.5" style="7"/>
+    <col min="9" max="9" width="49.42578125" customWidth="1"/>
+    <col min="10" max="10" width="27.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="11.42578125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:14" ht="18" x14ac:dyDescent="0.2">
       <c r="H1" s="4" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="H2" s="5">
         <v>44704</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="18"/>
       <c r="B3" s="18"/>
       <c r="C3" s="30"/>
@@ -2597,7 +2600,7 @@
       <c r="M3"/>
       <c r="N3" s="8"/>
     </row>
-    <row r="4" spans="1:14" s="37" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" s="37" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18"/>
       <c r="B4" s="18"/>
       <c r="C4" s="30"/>
@@ -2615,7 +2618,7 @@
       <c r="M4"/>
       <c r="N4" s="8"/>
     </row>
-    <row r="5" spans="1:14" s="37" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:14" s="37" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A5" s="18"/>
       <c r="B5" s="18"/>
       <c r="C5" s="30"/>
@@ -2631,7 +2634,7 @@
       <c r="M5"/>
       <c r="N5" s="8"/>
     </row>
-    <row r="6" spans="1:14" s="38" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:14" s="38" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
         <v>180</v>
       </c>
@@ -2675,7 +2678,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="32" t="s">
         <v>181</v>
       </c>
@@ -2720,7 +2723,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:14" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="32" t="s">
         <v>181</v>
       </c>
@@ -2759,7 +2762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:14" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="32" t="s">
         <v>181</v>
       </c>
@@ -2795,7 +2798,7 @@
       <c r="M9" s="46"/>
       <c r="N9" s="46"/>
     </row>
-    <row r="10" spans="1:14" s="43" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:14" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="32" t="s">
         <v>181</v>
       </c>
@@ -2834,7 +2837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="43" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:14" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="32" t="s">
         <v>181</v>
       </c>
@@ -2873,7 +2876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="43" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:14" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="32" t="s">
         <v>181</v>
       </c>
@@ -2912,7 +2915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:14" s="43" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:14" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="32" t="s">
         <v>181</v>
       </c>
@@ -2951,7 +2954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:14" s="43" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:14" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="32" t="s">
         <v>181</v>
       </c>
@@ -2990,7 +2993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:14" s="43" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:14" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="32" t="s">
         <v>181</v>
       </c>
@@ -3029,7 +3032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:14" s="43" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:14" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="32" t="s">
         <v>181</v>
       </c>
@@ -3068,7 +3071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:14" s="43" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:14" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="32" t="s">
         <v>181</v>
       </c>
@@ -3107,7 +3110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:14" s="43" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:14" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="32" t="s">
         <v>181</v>
       </c>
@@ -3146,7 +3149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:14" s="43" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:14" s="43" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A19" s="32" t="s">
         <v>181</v>
       </c>
@@ -3185,7 +3188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:14" s="43" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:14" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="32" t="s">
         <v>181</v>
       </c>
@@ -3224,7 +3227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:14" s="43" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:14" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="32" t="s">
         <v>181</v>
       </c>
@@ -3263,7 +3266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:14" s="43" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:14" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="32" t="s">
         <v>181</v>
       </c>
@@ -3302,7 +3305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:14" s="43" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:14" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="32" t="s">
         <v>181</v>
       </c>
@@ -3341,7 +3344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:14" s="43" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:14" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="32" t="s">
         <v>181</v>
       </c>
@@ -3380,7 +3383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:14" s="43" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:14" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="32" t="s">
         <v>181</v>
       </c>
@@ -3419,7 +3422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:14" s="43" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:14" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="32" t="s">
         <v>181</v>
       </c>
@@ -3458,7 +3461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:14" s="43" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:14" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="32" t="s">
         <v>181</v>
       </c>
@@ -3497,7 +3500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:14" s="43" customFormat="1" ht="56" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:14" s="43" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" s="32" t="s">
         <v>181</v>
       </c>
@@ -3536,7 +3539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:14" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:14" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="32" t="s">
         <v>181</v>
       </c>
@@ -3575,7 +3578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:14" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:14" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="32" t="s">
         <v>181</v>
       </c>
@@ -3614,7 +3617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:14" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:14" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="32" t="s">
         <v>181</v>
       </c>
@@ -3653,7 +3656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:14" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:14" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="32" t="s">
         <v>181</v>
       </c>
@@ -3692,7 +3695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:14" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:14" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" s="32" t="s">
         <v>181</v>
       </c>
@@ -3731,7 +3734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:14" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:14" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" s="32" t="s">
         <v>181</v>
       </c>
@@ -3770,7 +3773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:14" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:14" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="32" t="s">
         <v>181</v>
       </c>
@@ -3813,7 +3816,7 @@
         <v>1.24</v>
       </c>
     </row>
-    <row r="36" spans="1:14" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:14" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A36" s="32" t="s">
         <v>181</v>
       </c>
@@ -3858,7 +3861,7 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="37" spans="1:14" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:14" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" s="32" t="s">
         <v>181</v>
       </c>
@@ -3901,7 +3904,7 @@
         <v>2.96</v>
       </c>
     </row>
-    <row r="38" spans="1:14" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:14" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A38" s="32" t="s">
         <v>181</v>
       </c>
@@ -3946,7 +3949,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="39" spans="1:14" s="43" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:14" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="32" t="s">
         <v>181</v>
       </c>
@@ -3991,7 +3994,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="40" spans="1:14" s="43" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:14" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="32" t="s">
         <v>181</v>
       </c>
@@ -4034,7 +4037,7 @@
         <v>0.76</v>
       </c>
     </row>
-    <row r="41" spans="1:14" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:14" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" s="32" t="s">
         <v>181</v>
       </c>
@@ -4077,7 +4080,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="42" spans="1:14" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:14" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="32" t="s">
         <v>181</v>
       </c>
@@ -4120,7 +4123,7 @@
         <v>0.76</v>
       </c>
     </row>
-    <row r="43" spans="1:14" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:14" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A43" s="32" t="s">
         <v>181</v>
       </c>
@@ -4165,7 +4168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="32" t="s">
         <v>181</v>
       </c>
@@ -4208,7 +4211,7 @@
         <v>1.26</v>
       </c>
     </row>
-    <row r="45" spans="1:14" s="42" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:14" s="42" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A45" s="32" t="s">
         <v>181</v>
       </c>
@@ -4251,7 +4254,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="46" spans="1:14" s="42" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:14" s="42" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A46" s="32" t="s">
         <v>181</v>
       </c>
@@ -4294,7 +4297,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="47" spans="1:14" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:14" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A47" s="32" t="s">
         <v>181</v>
       </c>
@@ -4307,7 +4310,7 @@
       <c r="D47" s="34">
         <v>1</v>
       </c>
-      <c r="E47" s="35" t="s">
+      <c r="E47" s="98" t="s">
         <v>40</v>
       </c>
       <c r="F47" s="46" t="s">
@@ -4339,7 +4342,7 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="48" spans="1:14" s="42" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:14" s="42" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A48" s="32" t="s">
         <v>181</v>
       </c>
@@ -4382,7 +4385,7 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="49" spans="1:14" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:14" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A49" s="32" t="s">
         <v>181</v>
       </c>
@@ -4427,7 +4430,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="50" spans="1:14" s="43" customFormat="1" ht="16" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:14" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" s="32" t="s">
         <v>181</v>
       </c>
@@ -4470,7 +4473,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="51" spans="1:14" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:14" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A51" s="32" t="s">
         <v>181</v>
       </c>
@@ -4513,7 +4516,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="52" spans="1:14" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:14" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A52" s="32" t="s">
         <v>181</v>
       </c>
@@ -4556,7 +4559,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="53" spans="1:14" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:14" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A53" s="32" t="s">
         <v>181</v>
       </c>
@@ -4599,7 +4602,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="54" spans="1:14" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:14" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A54" s="32" t="s">
         <v>181</v>
       </c>
@@ -4642,7 +4645,7 @@
         <v>0.31</v>
       </c>
     </row>
-    <row r="55" spans="1:14" s="43" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:14" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="32" t="s">
         <v>181</v>
       </c>
@@ -4687,7 +4690,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="56" spans="1:14" s="43" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:14" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="32" t="s">
         <v>181</v>
       </c>
@@ -4730,7 +4733,7 @@
         <v>1.08</v>
       </c>
     </row>
-    <row r="57" spans="1:14" s="44" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:14" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="32" t="s">
         <v>181</v>
       </c>
@@ -4770,7 +4773,7 @@
       </c>
       <c r="N57" s="39"/>
     </row>
-    <row r="58" spans="1:14" s="44" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:14" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="32" t="s">
         <v>181</v>
       </c>
@@ -4804,7 +4807,7 @@
       <c r="M58" s="39"/>
       <c r="N58" s="39"/>
     </row>
-    <row r="59" spans="1:14" s="76" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:14" s="76" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="70" t="s">
         <v>255</v>
       </c>
@@ -4828,7 +4831,7 @@
       <c r="M59" s="73"/>
       <c r="N59" s="73"/>
     </row>
-    <row r="60" spans="1:14" s="76" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:14" s="76" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="70" t="s">
         <v>255</v>
       </c>
@@ -4852,7 +4855,7 @@
       <c r="M60" s="73"/>
       <c r="N60" s="73"/>
     </row>
-    <row r="61" spans="1:14" s="44" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:14" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="61" t="s">
         <v>118</v>
       </c>
@@ -4886,7 +4889,7 @@
       <c r="M61" s="39"/>
       <c r="N61" s="39"/>
     </row>
-    <row r="62" spans="1:14" s="44" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:14" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="61" t="s">
         <v>118</v>
       </c>
@@ -4920,7 +4923,7 @@
       <c r="M62" s="39"/>
       <c r="N62" s="39"/>
     </row>
-    <row r="63" spans="1:14" s="76" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:14" s="76" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="70" t="s">
         <v>255</v>
       </c>
@@ -4944,7 +4947,7 @@
       <c r="M63" s="73"/>
       <c r="N63" s="73"/>
     </row>
-    <row r="64" spans="1:14" s="76" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:14" s="76" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="70" t="s">
         <v>255</v>
       </c>
@@ -4968,7 +4971,7 @@
       <c r="M64" s="73"/>
       <c r="N64" s="73"/>
     </row>
-    <row r="65" spans="1:14" s="76" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:14" s="76" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="70" t="s">
         <v>255</v>
       </c>
@@ -4992,7 +4995,7 @@
       <c r="M65" s="73"/>
       <c r="N65" s="73"/>
     </row>
-    <row r="66" spans="1:14" s="76" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:14" s="76" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="70" t="s">
         <v>255</v>
       </c>
@@ -5016,7 +5019,7 @@
       <c r="M66" s="73"/>
       <c r="N66" s="73"/>
     </row>
-    <row r="67" spans="1:14" s="44" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:14" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="32" t="s">
         <v>181</v>
       </c>
@@ -5048,7 +5051,7 @@
       <c r="M67" s="39"/>
       <c r="N67" s="39"/>
     </row>
-    <row r="68" spans="1:14" s="76" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:14" s="76" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68" s="70" t="s">
         <v>255</v>
       </c>
@@ -5072,7 +5075,7 @@
       <c r="M68" s="73"/>
       <c r="N68" s="73"/>
     </row>
-    <row r="69" spans="1:14" s="76" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:14" s="76" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" s="70" t="s">
         <v>255</v>
       </c>
@@ -5096,7 +5099,7 @@
       <c r="M69" s="73"/>
       <c r="N69" s="73"/>
     </row>
-    <row r="70" spans="1:14" s="76" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:14" s="76" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" s="70" t="s">
         <v>255</v>
       </c>
@@ -5120,7 +5123,7 @@
       <c r="M70" s="73"/>
       <c r="N70" s="73"/>
     </row>
-    <row r="71" spans="1:14" s="43" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:14" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="32" t="s">
         <v>181</v>
       </c>
@@ -5156,7 +5159,7 @@
       <c r="M71" s="39"/>
       <c r="N71" s="39"/>
     </row>
-    <row r="72" spans="1:14" s="43" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:14" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="32" t="s">
         <v>181</v>
       </c>
@@ -5192,7 +5195,7 @@
       <c r="M72" s="39"/>
       <c r="N72" s="39"/>
     </row>
-    <row r="73" spans="1:14" s="43" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:14" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73" s="32" t="s">
         <v>181</v>
       </c>
@@ -5232,7 +5235,7 @@
       </c>
       <c r="N73" s="39"/>
     </row>
-    <row r="74" spans="1:14" s="44" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:14" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="61" t="s">
         <v>118</v>
       </c>
@@ -5268,7 +5271,7 @@
       <c r="M74" s="39"/>
       <c r="N74" s="39"/>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" s="32" t="s">
         <v>181</v>
       </c>
@@ -5304,7 +5307,7 @@
       <c r="M75" s="39"/>
       <c r="N75" s="39"/>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" s="32" t="s">
         <v>181</v>
       </c>
@@ -5340,7 +5343,7 @@
       <c r="M76" s="39"/>
       <c r="N76" s="39"/>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77" s="32" t="s">
         <v>181</v>
       </c>
@@ -5376,7 +5379,7 @@
       <c r="M77" s="39"/>
       <c r="N77" s="39"/>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" s="32" t="s">
         <v>181</v>
       </c>
@@ -5412,7 +5415,7 @@
       <c r="M78" s="39"/>
       <c r="N78" s="39"/>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79" s="32" t="s">
         <v>181</v>
       </c>
@@ -5450,7 +5453,7 @@
       <c r="M79" s="39"/>
       <c r="N79" s="39"/>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80" s="32" t="s">
         <v>181</v>
       </c>
@@ -5486,7 +5489,7 @@
       <c r="M80" s="39"/>
       <c r="N80" s="39"/>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81" s="32" t="s">
         <v>181</v>
       </c>
@@ -5522,7 +5525,7 @@
       <c r="M81" s="39"/>
       <c r="N81" s="39"/>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82" s="32" t="s">
         <v>181</v>
       </c>
@@ -5554,8 +5557,8 @@
       <c r="M82" s="39"/>
       <c r="N82" s="39"/>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="E86" s="97"/>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E86" s="94"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A7:B82">
@@ -5592,23 +5595,23 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="11.5" style="29"/>
-    <col min="4" max="4" width="60.5" customWidth="1"/>
+    <col min="1" max="2" width="11.42578125" style="29"/>
+    <col min="4" max="4" width="60.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="36" t="s">
         <v>191</v>
       </c>
       <c r="B1"/>
     </row>
-    <row r="2" spans="1:4" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2"/>
       <c r="B2"/>
     </row>
-    <row r="3" spans="1:4" s="26" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="27" t="s">
         <v>192</v>
       </c>
@@ -5622,7 +5625,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="79">
         <v>0</v>
       </c>
@@ -5636,7 +5639,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="70" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A5" s="82">
         <v>1</v>
       </c>
@@ -5650,7 +5653,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="28" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" s="82">
         <v>2</v>
       </c>
@@ -5664,7 +5667,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="82">
         <v>3</v>
       </c>
@@ -5678,17 +5681,17 @@
         <v>220</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="18" x14ac:dyDescent="0.15">
-      <c r="A8" s="94" t="s">
+    <row r="8" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A8" s="95" t="s">
         <v>268</v>
       </c>
-      <c r="B8" s="95"/>
-      <c r="C8" s="96"/>
+      <c r="B8" s="96"/>
+      <c r="C8" s="97"/>
       <c r="D8" s="87" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="252" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" ht="242.25" x14ac:dyDescent="0.2">
       <c r="A9" s="88">
         <v>1</v>
       </c>
@@ -5702,217 +5705,217 @@
         <v>267</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="88"/>
       <c r="B10" s="89"/>
       <c r="C10" s="92"/>
       <c r="D10" s="41"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="88"/>
       <c r="B11" s="89"/>
       <c r="C11" s="92"/>
       <c r="D11" s="22"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="88"/>
       <c r="B12" s="89"/>
       <c r="C12" s="92"/>
       <c r="D12" s="22"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="88"/>
       <c r="B13" s="89"/>
       <c r="C13" s="92"/>
       <c r="D13" s="22"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="88"/>
       <c r="B14" s="89"/>
       <c r="C14" s="92"/>
       <c r="D14" s="22"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="88"/>
       <c r="B15" s="89"/>
       <c r="C15" s="92"/>
       <c r="D15" s="22"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="88"/>
       <c r="B16" s="89"/>
       <c r="C16" s="92"/>
       <c r="D16" s="22"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="88"/>
       <c r="B17" s="89"/>
       <c r="C17" s="92"/>
       <c r="D17" s="22"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="88"/>
       <c r="B18" s="89"/>
       <c r="C18" s="92"/>
       <c r="D18" s="22"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="88"/>
       <c r="B19" s="89"/>
       <c r="C19" s="92"/>
       <c r="D19" s="22"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="88"/>
       <c r="B20" s="89"/>
       <c r="C20" s="92"/>
       <c r="D20" s="22"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="88"/>
       <c r="B21" s="89"/>
       <c r="C21" s="92"/>
       <c r="D21" s="22"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="88"/>
       <c r="B22" s="89"/>
       <c r="C22" s="92"/>
       <c r="D22" s="22"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="88"/>
       <c r="B23" s="89"/>
       <c r="C23" s="92"/>
       <c r="D23" s="22"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="88"/>
       <c r="B24" s="89"/>
       <c r="C24" s="92"/>
       <c r="D24" s="22"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="88"/>
       <c r="B25" s="89"/>
       <c r="C25" s="92"/>
       <c r="D25" s="22"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="88"/>
       <c r="B26" s="89"/>
       <c r="C26" s="92"/>
       <c r="D26" s="22"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="88"/>
       <c r="B27" s="89"/>
       <c r="C27" s="92"/>
       <c r="D27" s="22"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="88"/>
       <c r="B28" s="89"/>
       <c r="C28" s="92"/>
       <c r="D28" s="22"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="88"/>
       <c r="B29" s="89"/>
       <c r="C29" s="92"/>
       <c r="D29" s="22"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="88"/>
       <c r="B30" s="89"/>
       <c r="C30" s="92"/>
       <c r="D30" s="22"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="88"/>
       <c r="B31" s="89"/>
       <c r="C31" s="92"/>
       <c r="D31" s="22"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="88"/>
       <c r="B32" s="89"/>
       <c r="C32" s="92"/>
       <c r="D32" s="22"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="88"/>
       <c r="B33" s="89"/>
       <c r="C33" s="92"/>
       <c r="D33" s="22"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="88"/>
       <c r="B34" s="89"/>
       <c r="C34" s="92"/>
       <c r="D34" s="22"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="88"/>
       <c r="B35" s="89"/>
       <c r="C35" s="92"/>
       <c r="D35" s="22"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="88"/>
       <c r="B36" s="89"/>
       <c r="C36" s="92"/>
       <c r="D36" s="22"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="88"/>
       <c r="B37" s="89"/>
       <c r="C37" s="92"/>
       <c r="D37" s="22"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="88"/>
       <c r="B38" s="89"/>
       <c r="C38" s="92"/>
       <c r="D38" s="22"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="88"/>
       <c r="B39" s="89"/>
       <c r="C39" s="92"/>
       <c r="D39" s="22"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="88"/>
       <c r="B40" s="89"/>
       <c r="C40" s="92"/>
       <c r="D40" s="22"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="88"/>
       <c r="B41" s="89"/>
       <c r="C41" s="92"/>
       <c r="D41" s="22"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="88"/>
       <c r="B42" s="89"/>
       <c r="C42" s="92"/>
       <c r="D42" s="22"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="88"/>
       <c r="B43" s="89"/>
       <c r="C43" s="92"/>
       <c r="D43" s="22"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="88"/>
       <c r="B44" s="89"/>
       <c r="C44" s="92"/>
       <c r="D44" s="22"/>
     </row>
-    <row r="45" spans="1:4" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="90"/>
       <c r="B45" s="91"/>
       <c r="C45" s="93"/>

</xml_diff>